<commit_message>
add Spark related code
</commit_message>
<xml_diff>
--- a/resource/params_values_aws.xlsx
+++ b/resource/params_values_aws.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="changeable" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="358">
   <si>
     <t xml:space="preserve">Parameters</t>
   </si>
@@ -261,15 +261,6 @@
     <t xml:space="preserve">com.hadoop.compression.lzo.LzoCodec</t>
   </si>
   <si>
-    <t xml:space="preserve">io.compression.codecs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.apache.hadoop.io.compress.DefaultCodec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.apache.hadoop.io.compress.GzipCodec, org.apache.hadoop.io.compress.BZip2Codec, com.hadoop.compression.lzo.LzoCodec, com.hadoop.compression.lzo.LzopCodec</t>
-  </si>
-  <si>
     <t xml:space="preserve">io.file.buffer.size</t>
   </si>
   <si>
@@ -629,6 +620,12 @@
   </si>
   <si>
     <t xml:space="preserve">mapreduce.map.output.compress.codec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org.apache.hadoop.io.compress.DefaultCodec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org.apache.hadoop.io.compress.GzipCodec, org.apache.hadoop.io.compress.BZip2Codec, com.hadoop.compression.lzo.LzoCodec, com.hadoop.compression.lzo.LzopCodec</t>
   </si>
   <si>
     <t xml:space="preserve">mapreduce.map.skip.maxrecords</t>
@@ -1265,21 +1262,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E174"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C60" activeCellId="0" sqref="C60"/>
+      <selection pane="bottomLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="48.7295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="51.5663265306123"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="48.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,7 +1848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>79</v>
       </c>
@@ -1861,15 +1858,17 @@
       <c r="C46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="0"/>
+      <c r="D46" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="E46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="2" t="s">
         <v>83</v>
+      </c>
+      <c r="B47" s="2" t="n">
+        <v>128</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>84</v>
@@ -1879,12 +1878,12 @@
       </c>
       <c r="E47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>87</v>
@@ -1894,12 +1893,12 @@
       </c>
       <c r="E48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>90</v>
@@ -1909,48 +1908,48 @@
       </c>
       <c r="E49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="2" t="n">
+      <c r="B50" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+      <c r="E50" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="2" t="n">
         <v>1000000</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="C51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="E51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C51" s="0"/>
-      <c r="D51" s="0"/>
-      <c r="E51" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="2" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="C52" s="0"/>
       <c r="D52" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E52" s="0"/>
+      <c r="E52" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -1959,104 +1958,104 @@
       <c r="B53" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C53" s="0"/>
+      <c r="C53" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="D53" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="D54" s="0"/>
       <c r="E54" s="0"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="0"/>
+      <c r="C55" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="0"/>
+      <c r="E55" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="0"/>
-      <c r="E55" s="0"/>
-    </row>
-    <row r="56" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" s="0"/>
+      <c r="E56" s="0"/>
+    </row>
+    <row r="57" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="0"/>
-      <c r="C56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D56" s="0"/>
-      <c r="E56" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D57" s="0"/>
+      <c r="D57" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="E57" s="0"/>
     </row>
-    <row r="58" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D58" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="D58" s="0"/>
       <c r="E58" s="0"/>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D59" s="0"/>
       <c r="E59" s="0"/>
     </row>
-    <row r="60" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>120</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2064,22 +2063,20 @@
       </c>
       <c r="E60" s="0"/>
     </row>
-    <row r="61" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="D61" s="0"/>
       <c r="E61" s="0"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>125</v>
       </c>
@@ -2089,53 +2086,55 @@
       <c r="C62" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D62" s="0"/>
+      <c r="D62" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="E62" s="0"/>
     </row>
-    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D63" s="6" t="s">
         <v>131</v>
       </c>
+      <c r="D63" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E63" s="0"/>
     </row>
-    <row r="64" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D64" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="D64" s="0"/>
       <c r="E64" s="0"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D65" s="0"/>
       <c r="E65" s="0"/>
     </row>
-    <row r="66" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>139</v>
       </c>
@@ -2143,56 +2142,54 @@
         <v>68</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E66" s="0"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="B67" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="0"/>
+    </row>
+    <row r="68" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>134</v>
+      <c r="C68" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E68" s="0"/>
     </row>
-    <row r="69" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C69" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>149</v>
       </c>
+      <c r="D69" s="0"/>
       <c r="E69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,113 +2197,113 @@
         <v>150</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="0"/>
+      <c r="D70" s="0"/>
+      <c r="E70" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D70" s="0"/>
-      <c r="E70" s="0"/>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C71" s="0"/>
-      <c r="D71" s="0"/>
-      <c r="E71" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="D71" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E72" s="0"/>
     </row>
-    <row r="73" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E73" s="0"/>
     </row>
-    <row r="74" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>163</v>
+        <v>37</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D74" s="0"/>
+      <c r="E74" s="0"/>
+    </row>
+    <row r="75" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E74" s="0"/>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="C75" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D75" s="0"/>
+      <c r="D75" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="E75" s="0"/>
     </row>
-    <row r="76" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>168</v>
+        <v>19</v>
       </c>
       <c r="C76" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="E76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E76" s="0"/>
-    </row>
-    <row r="77" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C77" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D77" s="1" t="s">
         <v>172</v>
       </c>
+      <c r="D77" s="0"/>
       <c r="E77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,33 +2311,35 @@
         <v>173</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="D78" s="0"/>
       <c r="E78" s="0"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D79" s="0"/>
+      <c r="D79" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="E79" s="0"/>
     </row>
-    <row r="80" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>179</v>
+        <v>44</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>180</v>
@@ -2350,97 +2349,95 @@
       </c>
       <c r="E80" s="0"/>
     </row>
-    <row r="81" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D81" s="0"/>
+      <c r="E81" s="0"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E81" s="0"/>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="B82" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B82" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="6" t="s">
         <v>186</v>
       </c>
       <c r="D82" s="0"/>
       <c r="E82" s="0"/>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
         <v>187</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D83" s="0"/>
+      <c r="D83" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="E83" s="0"/>
     </row>
-    <row r="84" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B84" s="2" t="s">
         <v>191</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>1536</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>193</v>
-      </c>
+      <c r="D84" s="0"/>
       <c r="E84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B85" s="0" t="n">
-        <v>1536</v>
+        <v>193</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>195</v>
+        <v>37</v>
       </c>
       <c r="D85" s="0"/>
       <c r="E85" s="0"/>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D86" s="0"/>
       <c r="E86" s="0"/>
     </row>
-    <row r="87" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
         <v>197</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="D87" s="0"/>
       <c r="E87" s="0"/>
@@ -2450,40 +2447,40 @@
         <v>198</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="D88" s="0"/>
       <c r="E88" s="0"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
         <v>199</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E89" s="0"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D89" s="0"/>
-      <c r="E89" s="0"/>
-    </row>
-    <row r="90" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>203</v>
-      </c>
+      <c r="D90" s="0"/>
       <c r="E90" s="0"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2491,49 +2488,49 @@
         <v>204</v>
       </c>
       <c r="B91" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D91" s="0"/>
       <c r="E91" s="0"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
         <v>205</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>36</v>
+        <v>195</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="D92" s="0"/>
       <c r="E92" s="0"/>
     </row>
-    <row r="93" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
         <v>206</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>81</v>
+        <v>104</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="D93" s="0"/>
       <c r="E93" s="0"/>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="D94" s="0"/>
       <c r="E94" s="0"/>
@@ -2543,346 +2540,346 @@
         <v>208</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>19</v>
+        <v>209</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="D95" s="0"/>
       <c r="E95" s="0"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D96" s="0"/>
       <c r="E96" s="0"/>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D97" s="0"/>
+        <v>216</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="E97" s="0"/>
     </row>
-    <row r="98" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>218</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="D98" s="0"/>
       <c r="E98" s="0"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>191</v>
+        <v>221</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D99" s="0"/>
       <c r="E99" s="0"/>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>222</v>
+        <v>144</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D100" s="0"/>
       <c r="E100" s="0"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="D101" s="0"/>
       <c r="E101" s="0"/>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
         <v>226</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>147</v>
+        <v>227</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D102" s="0"/>
+        <v>228</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="E102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E103" s="0"/>
     </row>
-    <row r="104" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E104" s="0"/>
     </row>
-    <row r="105" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E105" s="0"/>
     </row>
-    <row r="106" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>240</v>
+        <v>126</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>242</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D106" s="0"/>
       <c r="E106" s="0"/>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
         <v>243</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>129</v>
+        <v>244</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="D107" s="0"/>
       <c r="E107" s="0"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>245</v>
+        <v>68</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D108" s="0"/>
+        <v>137</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="E108" s="0"/>
     </row>
-    <row r="109" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>247</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="D109" s="0"/>
       <c r="E109" s="0"/>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
         <v>248</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>68</v>
+        <v>249</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D110" s="0"/>
+        <v>250</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="E110" s="0"/>
     </row>
-    <row r="111" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>252</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="D111" s="0"/>
       <c r="E111" s="0"/>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E112" s="0"/>
+    </row>
+    <row r="113" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E113" s="0"/>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C112" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D112" s="0"/>
-      <c r="E112" s="0"/>
-    </row>
-    <row r="113" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E113" s="0"/>
-    </row>
-    <row r="114" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>263</v>
-      </c>
+      <c r="D114" s="0"/>
       <c r="E114" s="0"/>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
         <v>264</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D115" s="0"/>
+        <v>266</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="E115" s="0"/>
     </row>
-    <row r="116" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>268</v>
-      </c>
+      <c r="D116" s="0"/>
       <c r="E116" s="0"/>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
         <v>269</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D117" s="0"/>
       <c r="E117" s="0"/>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>271</v>
+        <v>130</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D118" s="0"/>
+        <v>174</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="E118" s="0"/>
     </row>
-    <row r="119" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>133</v>
+        <v>19</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>274</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="D119" s="0"/>
       <c r="E119" s="0"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,119 +2890,119 @@
         <v>19</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D120" s="0"/>
       <c r="E120" s="0"/>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
         <v>276</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>19</v>
+        <v>277</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>186</v>
+        <v>278</v>
       </c>
       <c r="D121" s="0"/>
       <c r="E121" s="0"/>
     </row>
-    <row r="122" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D122" s="0"/>
+        <v>281</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>282</v>
+      </c>
       <c r="E122" s="0"/>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>281</v>
+        <v>130</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>283</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D123" s="0"/>
       <c r="E123" s="0"/>
     </row>
-    <row r="124" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
         <v>284</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>133</v>
+        <v>270</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>177</v>
+        <v>285</v>
       </c>
       <c r="D124" s="0"/>
       <c r="E124" s="0"/>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D125" s="0"/>
       <c r="E125" s="0"/>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
+      </c>
+      <c r="B126" s="0" t="n">
+        <v>3072</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D126" s="0"/>
+        <v>222</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="E126" s="0"/>
     </row>
-    <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B127" s="0" t="n">
-        <v>3072</v>
+        <v>291</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>223</v>
+        <v>293</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>293</v>
+        <v>126</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>295</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D128" s="0"/>
       <c r="E128" s="0"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,93 +3010,92 @@
         <v>296</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D129" s="0"/>
       <c r="E129" s="0"/>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
         <v>297</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>129</v>
+        <v>298</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D130" s="0"/>
+        <v>299</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>300</v>
+      </c>
       <c r="E130" s="0"/>
     </row>
-    <row r="131" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E131" s="0"/>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E132" s="0"/>
     </row>
-    <row r="133" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>306</v>
+        <v>36</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>307</v>
+        <v>37</v>
       </c>
       <c r="E133" s="0"/>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>308</v>
       </c>
       <c r="B134" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C134" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E134" s="0"/>
-    </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E135" s="0"/>
+    </row>
+    <row r="136" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>312</v>
       </c>
@@ -3111,15 +3107,15 @@
       </c>
       <c r="E136" s="0"/>
     </row>
-    <row r="137" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
         <v>313</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="E137" s="0"/>
     </row>
@@ -3128,142 +3124,142 @@
         <v>314</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>19</v>
+        <v>315</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>186</v>
+        <v>316</v>
       </c>
       <c r="E138" s="0"/>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="E139" s="0"/>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>318</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>293</v>
+        <v>37</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>294</v>
+        <v>36</v>
       </c>
       <c r="E140" s="0"/>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>319</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>37</v>
+        <v>292</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>36</v>
+        <v>293</v>
       </c>
       <c r="E141" s="0"/>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
         <v>320</v>
       </c>
       <c r="B142" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E142" s="0"/>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C143" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C142" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E142" s="0"/>
-    </row>
-    <row r="143" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>323</v>
-      </c>
       <c r="E143" s="0"/>
     </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
         <v>324</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>293</v>
+        <v>325</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>294</v>
+        <v>326</v>
       </c>
       <c r="E144" s="0"/>
     </row>
-    <row r="145" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
+      </c>
+      <c r="B145" s="0" t="n">
+        <v>32</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E145" s="0"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>32</v>
+        <v>6144</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E146" s="0"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B147" s="0" t="n">
-        <v>6144</v>
+        <v>331</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>332</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E147" s="0"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E148" s="0"/>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>336</v>
+        <v>19</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>337</v>
+        <v>56</v>
       </c>
       <c r="E149" s="0"/>
     </row>
@@ -3284,10 +3280,10 @@
         <v>339</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>19</v>
+        <v>315</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>56</v>
+        <v>316</v>
       </c>
       <c r="E151" s="0"/>
     </row>
@@ -3296,71 +3292,71 @@
         <v>340</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>316</v>
+        <v>37</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>317</v>
+        <v>36</v>
       </c>
       <c r="E152" s="0"/>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E153" s="0"/>
+      <c r="B153" s="0" t="n">
+        <v>172800</v>
+      </c>
+      <c r="C153" s="0"/>
+      <c r="E153" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="s">
+      <c r="A154" s="0" t="s">
         <v>342</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>172800</v>
-      </c>
-      <c r="C154" s="0"/>
-      <c r="E154" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>67108864</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="E154" s="0"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>67108864</v>
-      </c>
-      <c r="C155" s="0" t="s">
-        <v>344</v>
+        <v>3600</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>345</v>
       </c>
       <c r="E155" s="0"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="B156" s="0" t="n">
-        <v>3600</v>
+        <v>346</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="E156" s="0"/>
+        <v>37</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>347</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C157" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="C157" s="0"/>
       <c r="E157" s="1" t="s">
         <v>8</v>
       </c>
@@ -3370,7 +3366,7 @@
         <v>348</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C158" s="0"/>
       <c r="E158" s="1" t="s">
@@ -3382,7 +3378,7 @@
         <v>349</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>36</v>
+        <v>350</v>
       </c>
       <c r="C159" s="0"/>
       <c r="E159" s="1" t="s">
@@ -3391,10 +3387,10 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="B160" s="2" t="s">
         <v>351</v>
+      </c>
+      <c r="B160" s="0" t="n">
+        <v>5000</v>
       </c>
       <c r="C160" s="0"/>
       <c r="E160" s="1" t="s">
@@ -3405,12 +3401,11 @@
       <c r="A161" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="B161" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="C161" s="0"/>
-      <c r="E161" s="1" t="s">
-        <v>8</v>
+      <c r="B161" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3418,35 +3413,25 @@
         <v>353</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>293</v>
+        <v>19</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>294</v>
+        <v>354</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>19</v>
+        <v>356</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="B164" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C164" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>